<commit_message>
Added a new tab to baravard.xlsx file
</commit_message>
<xml_diff>
--- a/baravard.xlsx
+++ b/baravard.xlsx
@@ -1,27 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\123\WebstormProjects\baravard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alissan\projects\baravard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E463ED3-0CC4-441A-8CE2-EB464F6E439C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDDDF55-FA26-40EE-89DC-919095EAD6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{9718141A-C964-469B-BF62-2E7A55EB37A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{9718141A-C964-469B-BF62-2E7A55EB37A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="توزین" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>بر آورد وزن اشیا</t>
+  </si>
+  <si>
+    <t>ردیف</t>
+  </si>
+  <si>
+    <t>نام</t>
+  </si>
+  <si>
+    <t>وزن</t>
+  </si>
+  <si>
+    <t>وزن کل</t>
+  </si>
+  <si>
+    <t>چمدان بزرگ</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -75,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -115,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -221,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -363,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -373,10 +408,182 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B8EC41-AAEB-492F-9AFD-0D69B12BA426}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3276B499-DD89-4769-8715-C5287AF1CAEF}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f>C3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" ref="D4:D23" si="0">C4+C3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
i changed some prices
</commit_message>
<xml_diff>
--- a/baravard.xlsx
+++ b/baravard.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\123\WebstormProjects\baravard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E463ED3-0CC4-441A-8CE2-EB464F6E439C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE347B-2094-4F6A-9D19-F3F802222ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{9718141A-C964-469B-BF62-2E7A55EB37A5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="برآورد هزینه" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,15 +24,49 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t xml:space="preserve">۴۵۸L یخچال شیاومی </t>
+  </si>
+  <si>
+    <t>تلویزیون هوشمند شیائومی 4s 4k</t>
+  </si>
+  <si>
+    <t>بلیت و اینا</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Baskerville Old Face"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Iranyekan"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,13 +86,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,12 +414,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B8EC41-AAEB-492F-9AFD-0D69B12BA426}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="31.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>45000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8000000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>